<commit_message>
Updated excel and added text file
Updated cloud_intervals_112024_D to include centerline data for all orbits 2-20 even and 15. I also added cloud_identifiaction_log_D which is a text document containing my personal notes detailing work I've done on this project.
</commit_message>
<xml_diff>
--- a/cloud_intervals_112024_D.xlsx
+++ b/cloud_intervals_112024_D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dallin\Documents\GitHub\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0469AA8-D1A3-45B4-9974-73A54930C70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A885352A-2B72-4276-900F-572B24A5105C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="10440" windowWidth="19380" windowHeight="10530" xr2:uid="{3AE738C0-3A1C-4DFE-88D2-21A5DEED96E6}"/>
+    <workbookView xWindow="11790" yWindow="470" windowWidth="28800" windowHeight="14010" xr2:uid="{3AE738C0-3A1C-4DFE-88D2-21A5DEED96E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Dallin" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Oribt #</t>
   </si>
@@ -80,9 +80,6 @@
     <t>15, 30, 45, …</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>awe_l1r_q20_2023326T0108_00002_v01.nc</t>
   </si>
   <si>
@@ -105,6 +102,23 @@
   </si>
   <si>
     <t>awe_l1r_q20_2023326T0108_00015_v01.nc</t>
+  </si>
+  <si>
+    <t>Start 
+(Center Column)</t>
+  </si>
+  <si>
+    <t>End 
+(Center Column)</t>
+  </si>
+  <si>
+    <t>awe_l1r_q20_2023326T0108_00016_v01.nc</t>
+  </si>
+  <si>
+    <t>awe_l1r_q20_2023326T0108_00018_v01.nc</t>
+  </si>
+  <si>
+    <t>awe_l1r_q20_2023326T0108_00020_v01.nc</t>
   </si>
 </sst>
 </file>
@@ -140,8 +154,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,19 +473,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47DEE03D-CE62-481C-AFCA-31D028C195CF}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E26" sqref="E25:E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="38.36328125" customWidth="1"/>
     <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="6" max="6" width="15.08984375" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,16 +503,19 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>1385</v>
@@ -505,7 +527,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D3">
         <v>934</v>
       </c>
@@ -513,12 +535,12 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>1406</v>
@@ -529,24 +551,42 @@
       <c r="E4">
         <v>514</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <v>912</v>
+      </c>
+      <c r="G4">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D5">
         <v>674</v>
       </c>
       <c r="E5">
         <v>877</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>941</v>
+      </c>
+      <c r="G5">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D6">
         <v>904</v>
       </c>
       <c r="E6">
         <v>1097</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <v>1194</v>
+      </c>
+      <c r="G6">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D7">
         <v>1110</v>
       </c>
@@ -554,12 +594,12 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>1425</v>
@@ -570,13 +610,19 @@
       <c r="E8">
         <v>1120</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <v>987</v>
+      </c>
+      <c r="G8">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>1410</v>
@@ -588,120 +634,323 @@
         <v>612</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D10">
         <v>951</v>
       </c>
       <c r="E10">
         <v>1192</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D11">
+      <c r="F10">
+        <v>1041</v>
+      </c>
+      <c r="G10">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <v>1060</v>
+      </c>
+      <c r="G11">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D12">
         <v>1301</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>1372</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D12">
+      <c r="F12">
+        <v>1313</v>
+      </c>
+      <c r="G12">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F13">
+        <v>1325</v>
+      </c>
+      <c r="G13">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D14">
         <v>1379</v>
       </c>
-      <c r="E12">
+      <c r="E14">
         <v>1410</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="F14">
+        <v>1410</v>
+      </c>
+      <c r="G14">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>1409</v>
+      </c>
+      <c r="D15">
+        <v>759</v>
+      </c>
+      <c r="E15">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D16">
+        <v>1081</v>
+      </c>
+      <c r="E16">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C13">
-        <v>1409</v>
-      </c>
-      <c r="D13">
-        <v>759</v>
-      </c>
-      <c r="E13">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D14">
-        <v>1081</v>
-      </c>
-      <c r="E14">
-        <v>1402</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C17">
+        <v>1404</v>
+      </c>
+      <c r="D17">
+        <v>989</v>
+      </c>
+      <c r="E17">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
         <v>20</v>
       </c>
-      <c r="C15">
-        <v>1404</v>
-      </c>
-      <c r="D15">
-        <v>989</v>
-      </c>
-      <c r="E15">
-        <v>1372</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C18">
+        <v>1406</v>
+      </c>
+      <c r="D18">
+        <v>1002</v>
+      </c>
+      <c r="E18">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D19">
+        <v>1253</v>
+      </c>
+      <c r="E19">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
         <v>21</v>
       </c>
-      <c r="C16">
+      <c r="C20">
+        <v>1405</v>
+      </c>
+      <c r="D20">
+        <v>1066</v>
+      </c>
+      <c r="E20">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D21">
+        <v>1337</v>
+      </c>
+      <c r="E21">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22">
         <v>1406</v>
       </c>
-      <c r="D16">
-        <v>1002</v>
-      </c>
-      <c r="E16">
-        <v>1180</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D17">
-        <v>1253</v>
-      </c>
-      <c r="E17">
-        <v>1384</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18">
-        <v>1405</v>
-      </c>
-      <c r="D18">
-        <v>1066</v>
-      </c>
-      <c r="E18">
-        <v>1240</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D19">
-        <v>1337</v>
-      </c>
-      <c r="E19">
-        <v>1405</v>
+      <c r="D22">
+        <v>982</v>
+      </c>
+      <c r="E22">
+        <v>1406</v>
+      </c>
+      <c r="F22">
+        <v>1015</v>
+      </c>
+      <c r="G22">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F23">
+        <v>1092</v>
+      </c>
+      <c r="G23">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F24">
+        <v>1160</v>
+      </c>
+      <c r="G24">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F25">
+        <v>1270</v>
+      </c>
+      <c r="G25">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F26">
+        <v>1331</v>
+      </c>
+      <c r="G26">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>18</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>1414</v>
+      </c>
+      <c r="D27">
+        <v>1414</v>
+      </c>
+      <c r="E27">
+        <v>1122</v>
+      </c>
+      <c r="F27">
+        <v>1122</v>
+      </c>
+      <c r="G27">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>1419</v>
+      </c>
+      <c r="D28">
+        <v>782</v>
+      </c>
+      <c r="E28">
+        <v>900</v>
+      </c>
+      <c r="F28">
+        <v>819</v>
+      </c>
+      <c r="G28">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D29">
+        <v>979</v>
+      </c>
+      <c r="E29">
+        <v>1192</v>
+      </c>
+      <c r="F29">
+        <v>1018</v>
+      </c>
+      <c r="G29">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F30">
+        <v>1038</v>
+      </c>
+      <c r="G30">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F31">
+        <v>1053</v>
+      </c>
+      <c r="G31">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F32">
+        <v>1074</v>
+      </c>
+      <c r="G32">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="F33">
+        <v>1145</v>
+      </c>
+      <c r="G33">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="34" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D34">
+        <v>1288</v>
+      </c>
+      <c r="E34">
+        <v>1419</v>
+      </c>
+      <c r="F34">
+        <v>1320</v>
+      </c>
+      <c r="G34">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="35" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="F35">
+        <v>1332</v>
+      </c>
+      <c r="G35">
+        <v>1419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ID complete for Orbits 22-44 even and 45
Cloud ID complete through for Orbits 2-44 even, 15, and 45. Daily log updated.
</commit_message>
<xml_diff>
--- a/cloud_intervals_112024_D.xlsx
+++ b/cloud_intervals_112024_D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dallin\Documents\GitHub\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A885352A-2B72-4276-900F-572B24A5105C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DF6C92-61C2-4EAE-8A7F-AED1B2216614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11790" yWindow="470" windowWidth="28800" windowHeight="14010" xr2:uid="{3AE738C0-3A1C-4DFE-88D2-21A5DEED96E6}"/>
+    <workbookView xWindow="7500" yWindow="15240" windowWidth="30990" windowHeight="5730" xr2:uid="{3AE738C0-3A1C-4DFE-88D2-21A5DEED96E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Dallin" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Oribt #</t>
   </si>
@@ -119,6 +119,45 @@
   </si>
   <si>
     <t>awe_l1r_q20_2023326T0108_00020_v01.nc</t>
+  </si>
+  <si>
+    <t>awe_l1r_q20_2023326T0108_00022_v01.nc</t>
+  </si>
+  <si>
+    <t>awe_l1r_q20_2023326T0108_00024_v01.nc</t>
+  </si>
+  <si>
+    <t>awe_l1r_q20_2023326T0108_00026_v01.nc</t>
+  </si>
+  <si>
+    <t>awe_l1r_q20_2023326T0108_00028_v01.nc</t>
+  </si>
+  <si>
+    <t>awe_l1r_q20_2023326T0108_00030_v01.nc</t>
+  </si>
+  <si>
+    <t>awe_l1r_q20_2023326T0108_00034_v01.nc</t>
+  </si>
+  <si>
+    <t>awe_l1r_q20_2023326T0108_00032_v01.nc</t>
+  </si>
+  <si>
+    <t>awe_l1r_q20_2023326T0108_00036_v01.nc</t>
+  </si>
+  <si>
+    <t>awe_l1r_q20_2023326T0108_00038_v01.nc</t>
+  </si>
+  <si>
+    <t>awe_l1r_q20_2023326T0108_00040_v01.nc</t>
+  </si>
+  <si>
+    <t>awe_l1r_q20_2023326T0108_00042_v01.nc</t>
+  </si>
+  <si>
+    <t>awe_l1r_q20_2023326T0108_00044_v01.nc</t>
+  </si>
+  <si>
+    <t>awe_l1r_q20_2023326T0108_00045_v01.nc</t>
   </si>
 </sst>
 </file>
@@ -473,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47DEE03D-CE62-481C-AFCA-31D028C195CF}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -923,7 +962,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F33">
         <v>1145</v>
       </c>
@@ -931,7 +970,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D34">
         <v>1288</v>
       </c>
@@ -945,12 +984,711 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F35">
         <v>1332</v>
       </c>
       <c r="G35">
         <v>1419</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36">
+        <v>1432</v>
+      </c>
+      <c r="D36">
+        <v>558</v>
+      </c>
+      <c r="E36">
+        <v>756</v>
+      </c>
+      <c r="F36">
+        <v>596</v>
+      </c>
+      <c r="G36">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F37">
+        <v>695</v>
+      </c>
+      <c r="G37">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D38">
+        <v>992</v>
+      </c>
+      <c r="E38">
+        <v>1112</v>
+      </c>
+      <c r="F38">
+        <v>1030</v>
+      </c>
+      <c r="G38">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>24</v>
+      </c>
+      <c r="B39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39">
+        <v>1424</v>
+      </c>
+      <c r="D39">
+        <v>948</v>
+      </c>
+      <c r="E39">
+        <v>1390</v>
+      </c>
+      <c r="F39">
+        <v>978</v>
+      </c>
+      <c r="G39">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F40">
+        <v>1066</v>
+      </c>
+      <c r="G40">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F41">
+        <v>1158</v>
+      </c>
+      <c r="G41">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F42">
+        <v>1186</v>
+      </c>
+      <c r="G42">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F43">
+        <v>1337</v>
+      </c>
+      <c r="G43">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>26</v>
+      </c>
+      <c r="B44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44">
+        <v>1444</v>
+      </c>
+      <c r="D44">
+        <v>809</v>
+      </c>
+      <c r="E44">
+        <v>1296</v>
+      </c>
+      <c r="F44">
+        <v>847</v>
+      </c>
+      <c r="G44">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F45">
+        <v>972</v>
+      </c>
+      <c r="G45">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F46">
+        <v>1078</v>
+      </c>
+      <c r="G46">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F47">
+        <v>1131</v>
+      </c>
+      <c r="G47">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F48">
+        <v>1242</v>
+      </c>
+      <c r="G48">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>28</v>
+      </c>
+      <c r="B49" t="s">
+        <v>30</v>
+      </c>
+      <c r="C49">
+        <v>1442</v>
+      </c>
+      <c r="D49">
+        <v>862</v>
+      </c>
+      <c r="E49">
+        <v>1173</v>
+      </c>
+      <c r="F49">
+        <v>889</v>
+      </c>
+      <c r="G49">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F50">
+        <v>977</v>
+      </c>
+      <c r="G50">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F51">
+        <v>1001</v>
+      </c>
+      <c r="G51">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F52">
+        <v>1018</v>
+      </c>
+      <c r="G52">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F53">
+        <v>1112</v>
+      </c>
+      <c r="G53">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>30</v>
+      </c>
+      <c r="B54" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54">
+        <v>1461</v>
+      </c>
+      <c r="D54">
+        <v>170</v>
+      </c>
+      <c r="E54">
+        <v>236</v>
+      </c>
+      <c r="F54">
+        <v>191</v>
+      </c>
+      <c r="G54">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D55">
+        <v>448</v>
+      </c>
+      <c r="E55">
+        <v>537</v>
+      </c>
+      <c r="F55">
+        <v>488</v>
+      </c>
+      <c r="G55">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D56">
+        <v>1013</v>
+      </c>
+      <c r="E56">
+        <v>1300</v>
+      </c>
+      <c r="F56">
+        <v>1054</v>
+      </c>
+      <c r="G56">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F57">
+        <v>1104</v>
+      </c>
+      <c r="G57">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F58">
+        <v>1205</v>
+      </c>
+      <c r="G58">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>32</v>
+      </c>
+      <c r="B59" t="s">
+        <v>33</v>
+      </c>
+      <c r="C59">
+        <v>1460</v>
+      </c>
+      <c r="D59">
+        <v>438</v>
+      </c>
+      <c r="E59">
+        <v>580</v>
+      </c>
+      <c r="F59">
+        <v>473</v>
+      </c>
+      <c r="G59">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>34</v>
+      </c>
+      <c r="B60" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60">
+        <v>1483</v>
+      </c>
+      <c r="D60">
+        <v>188</v>
+      </c>
+      <c r="E60">
+        <v>270</v>
+      </c>
+      <c r="F60">
+        <v>211</v>
+      </c>
+      <c r="G60">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D61">
+        <v>403</v>
+      </c>
+      <c r="E61">
+        <v>519</v>
+      </c>
+      <c r="F61">
+        <v>431</v>
+      </c>
+      <c r="G61">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D62">
+        <v>999</v>
+      </c>
+      <c r="E62">
+        <v>1186</v>
+      </c>
+      <c r="F62">
+        <v>1021</v>
+      </c>
+      <c r="G62">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F63">
+        <v>1076</v>
+      </c>
+      <c r="G63">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F64">
+        <v>1113</v>
+      </c>
+      <c r="G64">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F65">
+        <v>1140</v>
+      </c>
+      <c r="G65">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D66">
+        <v>1320</v>
+      </c>
+      <c r="E66">
+        <v>1483</v>
+      </c>
+      <c r="F66">
+        <v>1357</v>
+      </c>
+      <c r="G66">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F67">
+        <v>1376</v>
+      </c>
+      <c r="G67">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F68">
+        <v>1448</v>
+      </c>
+      <c r="G68">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>36</v>
+      </c>
+      <c r="B69" t="s">
+        <v>34</v>
+      </c>
+      <c r="C69">
+        <v>1482</v>
+      </c>
+      <c r="D69">
+        <v>288</v>
+      </c>
+      <c r="E69">
+        <v>387</v>
+      </c>
+      <c r="F69">
+        <v>327</v>
+      </c>
+      <c r="G69">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D70">
+        <v>872</v>
+      </c>
+      <c r="E70">
+        <v>984</v>
+      </c>
+      <c r="F70">
+        <v>905</v>
+      </c>
+      <c r="G70">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F71">
+        <v>927</v>
+      </c>
+      <c r="G71">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>38</v>
+      </c>
+      <c r="B72" t="s">
+        <v>35</v>
+      </c>
+      <c r="C72">
+        <v>1492</v>
+      </c>
+      <c r="D72">
+        <v>555</v>
+      </c>
+      <c r="E72">
+        <v>598</v>
+      </c>
+      <c r="F72">
+        <v>650</v>
+      </c>
+      <c r="G72">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>40</v>
+      </c>
+      <c r="B73" t="s">
+        <v>36</v>
+      </c>
+      <c r="C73">
+        <v>1479</v>
+      </c>
+      <c r="D73">
+        <v>977</v>
+      </c>
+      <c r="E73">
+        <v>1433</v>
+      </c>
+      <c r="F73">
+        <v>1007</v>
+      </c>
+      <c r="G73">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F74">
+        <v>1027</v>
+      </c>
+      <c r="G74">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F75">
+        <v>1233</v>
+      </c>
+      <c r="G75">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F76">
+        <v>1295</v>
+      </c>
+      <c r="G76">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F77">
+        <v>1308</v>
+      </c>
+      <c r="G77">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F78">
+        <v>1330</v>
+      </c>
+      <c r="G78">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F79">
+        <v>1357</v>
+      </c>
+      <c r="G79">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>42</v>
+      </c>
+      <c r="B80" t="s">
+        <v>37</v>
+      </c>
+      <c r="C80">
+        <v>1492</v>
+      </c>
+      <c r="D80">
+        <v>906</v>
+      </c>
+      <c r="E80">
+        <v>1343</v>
+      </c>
+      <c r="F80">
+        <v>930</v>
+      </c>
+      <c r="G80">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F81">
+        <v>960</v>
+      </c>
+      <c r="G81">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F82">
+        <v>1034</v>
+      </c>
+      <c r="G82">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F83">
+        <v>1148</v>
+      </c>
+      <c r="G83">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F84">
+        <v>1209</v>
+      </c>
+      <c r="G84">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F85">
+        <v>1293</v>
+      </c>
+      <c r="G85">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>44</v>
+      </c>
+      <c r="B86" t="s">
+        <v>38</v>
+      </c>
+      <c r="C86">
+        <v>1481</v>
+      </c>
+      <c r="D86">
+        <v>285</v>
+      </c>
+      <c r="E86">
+        <v>380</v>
+      </c>
+      <c r="F86">
+        <v>318</v>
+      </c>
+      <c r="G86">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D87">
+        <v>948</v>
+      </c>
+      <c r="E87">
+        <v>1230</v>
+      </c>
+      <c r="F87">
+        <v>985</v>
+      </c>
+      <c r="G87">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F88">
+        <v>1027</v>
+      </c>
+      <c r="G88">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F89">
+        <v>1045</v>
+      </c>
+      <c r="G89">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>45</v>
+      </c>
+      <c r="B90" t="s">
+        <v>39</v>
+      </c>
+      <c r="C90">
+        <v>1497</v>
+      </c>
+      <c r="D90">
+        <v>1068</v>
+      </c>
+      <c r="E90">
+        <v>1347</v>
+      </c>
+      <c r="F90">
+        <v>1094</v>
+      </c>
+      <c r="G90">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F91">
+        <v>1166</v>
+      </c>
+      <c r="G91">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F92">
+        <v>1204</v>
+      </c>
+      <c r="G92">
+        <v>1286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>